<commit_message>
run three models seperately
</commit_message>
<xml_diff>
--- a/accuracies.xlsx
+++ b/accuracies.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D21"/>
+  <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -449,24 +449,16 @@
           <t>Author Accuracy</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>Combined Accuracy</t>
-        </is>
-      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
         <v>1</v>
       </c>
       <c r="B2" t="n">
-        <v>58.33333333333334</v>
+        <v>39</v>
       </c>
       <c r="C2" t="n">
-        <v>65.66666666666667</v>
-      </c>
-      <c r="D2" t="n">
-        <v>62</v>
+        <v>23.83333333333333</v>
       </c>
     </row>
     <row r="3">
@@ -474,13 +466,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="n">
-        <v>85.33333333333333</v>
+        <v>58.66666666666666</v>
       </c>
       <c r="C3" t="n">
-        <v>72.5</v>
-      </c>
-      <c r="D3" t="n">
-        <v>78.91666666666666</v>
+        <v>12.66666666666667</v>
       </c>
     </row>
     <row r="4">
@@ -488,13 +477,10 @@
         <v>3</v>
       </c>
       <c r="B4" t="n">
-        <v>91.66666666666667</v>
+        <v>77.83333333333333</v>
       </c>
       <c r="C4" t="n">
-        <v>77.16666666666667</v>
-      </c>
-      <c r="D4" t="n">
-        <v>84.41666666666667</v>
+        <v>20.66666666666667</v>
       </c>
     </row>
     <row r="5">
@@ -502,13 +488,10 @@
         <v>4</v>
       </c>
       <c r="B5" t="n">
-        <v>92.66666666666667</v>
+        <v>86.16666666666667</v>
       </c>
       <c r="C5" t="n">
-        <v>81.66666666666667</v>
-      </c>
-      <c r="D5" t="n">
-        <v>87.16666666666667</v>
+        <v>22.5</v>
       </c>
     </row>
     <row r="6">
@@ -516,13 +499,10 @@
         <v>5</v>
       </c>
       <c r="B6" t="n">
-        <v>94.5</v>
+        <v>88.83333333333333</v>
       </c>
       <c r="C6" t="n">
-        <v>83.33333333333333</v>
-      </c>
-      <c r="D6" t="n">
-        <v>88.91666666666666</v>
+        <v>22</v>
       </c>
     </row>
     <row r="7">
@@ -530,13 +510,10 @@
         <v>6</v>
       </c>
       <c r="B7" t="n">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="C7" t="n">
-        <v>84.83333333333333</v>
-      </c>
-      <c r="D7" t="n">
-        <v>89.41666666666666</v>
+        <v>24.66666666666667</v>
       </c>
     </row>
     <row r="8">
@@ -544,13 +521,10 @@
         <v>7</v>
       </c>
       <c r="B8" t="n">
-        <v>94.5</v>
+        <v>90.83333333333333</v>
       </c>
       <c r="C8" t="n">
-        <v>84</v>
-      </c>
-      <c r="D8" t="n">
-        <v>89.25</v>
+        <v>21.66666666666667</v>
       </c>
     </row>
     <row r="9">
@@ -558,13 +532,10 @@
         <v>8</v>
       </c>
       <c r="B9" t="n">
-        <v>94.66666666666667</v>
+        <v>92.16666666666667</v>
       </c>
       <c r="C9" t="n">
-        <v>85.66666666666667</v>
-      </c>
-      <c r="D9" t="n">
-        <v>90.16666666666667</v>
+        <v>22.83333333333333</v>
       </c>
     </row>
     <row r="10">
@@ -572,13 +543,10 @@
         <v>9</v>
       </c>
       <c r="B10" t="n">
-        <v>94.66666666666667</v>
+        <v>91.83333333333333</v>
       </c>
       <c r="C10" t="n">
-        <v>85.5</v>
-      </c>
-      <c r="D10" t="n">
-        <v>90.08333333333334</v>
+        <v>22.33333333333333</v>
       </c>
     </row>
     <row r="11">
@@ -586,13 +554,10 @@
         <v>10</v>
       </c>
       <c r="B11" t="n">
-        <v>95.16666666666667</v>
+        <v>91.83333333333333</v>
       </c>
       <c r="C11" t="n">
-        <v>85.33333333333333</v>
-      </c>
-      <c r="D11" t="n">
-        <v>90.25</v>
+        <v>22.16666666666667</v>
       </c>
     </row>
     <row r="12">
@@ -600,13 +565,10 @@
         <v>11</v>
       </c>
       <c r="B12" t="n">
-        <v>95.16666666666667</v>
+        <v>92</v>
       </c>
       <c r="C12" t="n">
-        <v>85.83333333333333</v>
-      </c>
-      <c r="D12" t="n">
-        <v>90.5</v>
+        <v>22.16666666666667</v>
       </c>
     </row>
     <row r="13">
@@ -614,13 +576,10 @@
         <v>12</v>
       </c>
       <c r="B13" t="n">
-        <v>95.16666666666667</v>
+        <v>92.33333333333333</v>
       </c>
       <c r="C13" t="n">
-        <v>85</v>
-      </c>
-      <c r="D13" t="n">
-        <v>90.08333333333334</v>
+        <v>22.66666666666667</v>
       </c>
     </row>
     <row r="14">
@@ -628,13 +587,10 @@
         <v>13</v>
       </c>
       <c r="B14" t="n">
-        <v>95.5</v>
+        <v>92.33333333333333</v>
       </c>
       <c r="C14" t="n">
-        <v>85.66666666666667</v>
-      </c>
-      <c r="D14" t="n">
-        <v>90.58333333333334</v>
+        <v>21.83333333333333</v>
       </c>
     </row>
     <row r="15">
@@ -642,13 +598,10 @@
         <v>14</v>
       </c>
       <c r="B15" t="n">
-        <v>95.33333333333333</v>
+        <v>92.33333333333333</v>
       </c>
       <c r="C15" t="n">
-        <v>86</v>
-      </c>
-      <c r="D15" t="n">
-        <v>90.66666666666666</v>
+        <v>22.33333333333333</v>
       </c>
     </row>
     <row r="16">
@@ -656,13 +609,10 @@
         <v>15</v>
       </c>
       <c r="B16" t="n">
-        <v>95.33333333333333</v>
+        <v>92.16666666666667</v>
       </c>
       <c r="C16" t="n">
-        <v>85.5</v>
-      </c>
-      <c r="D16" t="n">
-        <v>90.41666666666666</v>
+        <v>21.66666666666667</v>
       </c>
     </row>
     <row r="17">
@@ -670,13 +620,10 @@
         <v>16</v>
       </c>
       <c r="B17" t="n">
-        <v>95.33333333333333</v>
+        <v>92.33333333333333</v>
       </c>
       <c r="C17" t="n">
-        <v>85.83333333333333</v>
-      </c>
-      <c r="D17" t="n">
-        <v>90.58333333333333</v>
+        <v>21.83333333333333</v>
       </c>
     </row>
     <row r="18">
@@ -684,13 +631,10 @@
         <v>17</v>
       </c>
       <c r="B18" t="n">
-        <v>95.5</v>
+        <v>92.33333333333333</v>
       </c>
       <c r="C18" t="n">
-        <v>85.66666666666667</v>
-      </c>
-      <c r="D18" t="n">
-        <v>90.58333333333334</v>
+        <v>21.83333333333333</v>
       </c>
     </row>
     <row r="19">
@@ -698,13 +642,10 @@
         <v>18</v>
       </c>
       <c r="B19" t="n">
-        <v>95.5</v>
+        <v>92.5</v>
       </c>
       <c r="C19" t="n">
-        <v>85.66666666666667</v>
-      </c>
-      <c r="D19" t="n">
-        <v>90.58333333333334</v>
+        <v>21.83333333333333</v>
       </c>
     </row>
     <row r="20">
@@ -712,13 +653,10 @@
         <v>19</v>
       </c>
       <c r="B20" t="n">
-        <v>95.5</v>
+        <v>92.5</v>
       </c>
       <c r="C20" t="n">
-        <v>85.83333333333333</v>
-      </c>
-      <c r="D20" t="n">
-        <v>90.66666666666666</v>
+        <v>21.66666666666667</v>
       </c>
     </row>
     <row r="21">
@@ -726,13 +664,10 @@
         <v>20</v>
       </c>
       <c r="B21" t="n">
-        <v>95.5</v>
+        <v>92.5</v>
       </c>
       <c r="C21" t="n">
-        <v>85.83333333333333</v>
-      </c>
-      <c r="D21" t="n">
-        <v>90.66666666666666</v>
+        <v>21.66666666666667</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
modify three models to three excels
</commit_message>
<xml_diff>
--- a/accuracies.xlsx
+++ b/accuracies.xlsx
@@ -441,12 +441,12 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Digit Accuracy</t>
+          <t>Digit Accuracy (Author)</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Author Accuracy</t>
+          <t>Author Accuracy (Author)</t>
         </is>
       </c>
     </row>
@@ -455,10 +455,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="n">
-        <v>39</v>
+        <v>12.16666666666667</v>
       </c>
       <c r="C2" t="n">
-        <v>23.83333333333333</v>
+        <v>64.33333333333333</v>
       </c>
     </row>
     <row r="3">
@@ -466,10 +466,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="n">
-        <v>58.66666666666666</v>
+        <v>11.16666666666667</v>
       </c>
       <c r="C3" t="n">
-        <v>12.66666666666667</v>
+        <v>68.83333333333333</v>
       </c>
     </row>
     <row r="4">
@@ -477,10 +477,10 @@
         <v>3</v>
       </c>
       <c r="B4" t="n">
-        <v>77.83333333333333</v>
+        <v>11.33333333333333</v>
       </c>
       <c r="C4" t="n">
-        <v>20.66666666666667</v>
+        <v>74.16666666666667</v>
       </c>
     </row>
     <row r="5">
@@ -488,10 +488,10 @@
         <v>4</v>
       </c>
       <c r="B5" t="n">
-        <v>86.16666666666667</v>
+        <v>12.33333333333333</v>
       </c>
       <c r="C5" t="n">
-        <v>22.5</v>
+        <v>73.66666666666667</v>
       </c>
     </row>
     <row r="6">
@@ -499,10 +499,10 @@
         <v>5</v>
       </c>
       <c r="B6" t="n">
-        <v>88.83333333333333</v>
+        <v>12.66666666666667</v>
       </c>
       <c r="C6" t="n">
-        <v>22</v>
+        <v>74.83333333333333</v>
       </c>
     </row>
     <row r="7">
@@ -510,10 +510,10 @@
         <v>6</v>
       </c>
       <c r="B7" t="n">
-        <v>89</v>
+        <v>10.83333333333333</v>
       </c>
       <c r="C7" t="n">
-        <v>24.66666666666667</v>
+        <v>76</v>
       </c>
     </row>
     <row r="8">
@@ -521,10 +521,10 @@
         <v>7</v>
       </c>
       <c r="B8" t="n">
-        <v>90.83333333333333</v>
+        <v>12.16666666666667</v>
       </c>
       <c r="C8" t="n">
-        <v>21.66666666666667</v>
+        <v>76.33333333333333</v>
       </c>
     </row>
     <row r="9">
@@ -532,10 +532,10 @@
         <v>8</v>
       </c>
       <c r="B9" t="n">
-        <v>92.16666666666667</v>
+        <v>11.33333333333333</v>
       </c>
       <c r="C9" t="n">
-        <v>22.83333333333333</v>
+        <v>75.66666666666667</v>
       </c>
     </row>
     <row r="10">
@@ -543,10 +543,10 @@
         <v>9</v>
       </c>
       <c r="B10" t="n">
-        <v>91.83333333333333</v>
+        <v>11.16666666666667</v>
       </c>
       <c r="C10" t="n">
-        <v>22.33333333333333</v>
+        <v>75.66666666666667</v>
       </c>
     </row>
     <row r="11">
@@ -554,10 +554,10 @@
         <v>10</v>
       </c>
       <c r="B11" t="n">
-        <v>91.83333333333333</v>
+        <v>11.5</v>
       </c>
       <c r="C11" t="n">
-        <v>22.16666666666667</v>
+        <v>76.33333333333333</v>
       </c>
     </row>
     <row r="12">
@@ -565,10 +565,10 @@
         <v>11</v>
       </c>
       <c r="B12" t="n">
-        <v>92</v>
+        <v>11.16666666666667</v>
       </c>
       <c r="C12" t="n">
-        <v>22.16666666666667</v>
+        <v>76.66666666666667</v>
       </c>
     </row>
     <row r="13">
@@ -576,10 +576,10 @@
         <v>12</v>
       </c>
       <c r="B13" t="n">
-        <v>92.33333333333333</v>
+        <v>11.33333333333333</v>
       </c>
       <c r="C13" t="n">
-        <v>22.66666666666667</v>
+        <v>76.16666666666667</v>
       </c>
     </row>
     <row r="14">
@@ -587,10 +587,10 @@
         <v>13</v>
       </c>
       <c r="B14" t="n">
-        <v>92.33333333333333</v>
+        <v>11.66666666666667</v>
       </c>
       <c r="C14" t="n">
-        <v>21.83333333333333</v>
+        <v>76.83333333333333</v>
       </c>
     </row>
     <row r="15">
@@ -598,10 +598,10 @@
         <v>14</v>
       </c>
       <c r="B15" t="n">
-        <v>92.33333333333333</v>
+        <v>11.5</v>
       </c>
       <c r="C15" t="n">
-        <v>22.33333333333333</v>
+        <v>76.5</v>
       </c>
     </row>
     <row r="16">
@@ -609,10 +609,10 @@
         <v>15</v>
       </c>
       <c r="B16" t="n">
-        <v>92.16666666666667</v>
+        <v>11.83333333333333</v>
       </c>
       <c r="C16" t="n">
-        <v>21.66666666666667</v>
+        <v>76.83333333333333</v>
       </c>
     </row>
     <row r="17">
@@ -620,10 +620,10 @@
         <v>16</v>
       </c>
       <c r="B17" t="n">
-        <v>92.33333333333333</v>
+        <v>11.5</v>
       </c>
       <c r="C17" t="n">
-        <v>21.83333333333333</v>
+        <v>76.66666666666667</v>
       </c>
     </row>
     <row r="18">
@@ -631,10 +631,10 @@
         <v>17</v>
       </c>
       <c r="B18" t="n">
-        <v>92.33333333333333</v>
+        <v>11.66666666666667</v>
       </c>
       <c r="C18" t="n">
-        <v>21.83333333333333</v>
+        <v>76.83333333333333</v>
       </c>
     </row>
     <row r="19">
@@ -642,10 +642,10 @@
         <v>18</v>
       </c>
       <c r="B19" t="n">
-        <v>92.5</v>
+        <v>11.66666666666667</v>
       </c>
       <c r="C19" t="n">
-        <v>21.83333333333333</v>
+        <v>76.83333333333333</v>
       </c>
     </row>
     <row r="20">
@@ -653,10 +653,10 @@
         <v>19</v>
       </c>
       <c r="B20" t="n">
-        <v>92.5</v>
+        <v>11.66666666666667</v>
       </c>
       <c r="C20" t="n">
-        <v>21.66666666666667</v>
+        <v>76.83333333333333</v>
       </c>
     </row>
     <row r="21">
@@ -664,10 +664,10 @@
         <v>20</v>
       </c>
       <c r="B21" t="n">
-        <v>92.5</v>
+        <v>11.66666666666667</v>
       </c>
       <c r="C21" t="n">
-        <v>21.66666666666667</v>
+        <v>76.66666666666667</v>
       </c>
     </row>
   </sheetData>

</xml_diff>